<commit_message>
added command to drop rows that are NA
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (PP)/H4Sci_RPackage/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D9E9C9-484C-494C-8FAB-8128DE9350D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E340869A-3D66-2C4C-8A01-A05CAFBE7EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-9660" windowWidth="12800" windowHeight="23500" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="29400" yWindow="-1980" windowWidth="12800" windowHeight="21100" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
   <si>
     <t>NNSS</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>Brunner</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -203,10 +206,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -506,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -689,6 +688,16 @@
         <v>20000</v>
       </c>
     </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="3">
+        <v>7560000000004</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Changed some ahv-nr to include cases we want to detect with new ahv_format variable
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E340869A-3D66-2C4C-8A01-A05CAFBE7EBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F985A1F6-DA54-6B41-930C-3F1383FE14F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-1980" windowWidth="12800" windowHeight="21100" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="29400" yWindow="-7260" windowWidth="23560" windowHeight="21100" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>NNSS</t>
   </si>
@@ -135,6 +135,33 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>756AB00000004</t>
+  </si>
+  <si>
+    <t>7230000XYZ</t>
+  </si>
+  <si>
+    <t>Dachs</t>
+  </si>
+  <si>
+    <t>Dario</t>
+  </si>
+  <si>
+    <t>Eris</t>
+  </si>
+  <si>
+    <t>Elsa</t>
+  </si>
+  <si>
+    <t>Fiona</t>
+  </si>
+  <si>
+    <t>Fichter</t>
+  </si>
+  <si>
+    <t>756.0000.000.004</t>
   </si>
 </sst>
 </file>
@@ -505,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -694,8 +721,36 @@
       </c>
     </row>
     <row r="6" spans="1:14">
-      <c r="A6" s="3">
-        <v>7560000000004</v>
+      <c r="A6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saves ahv-nr as character to make keytable columns robust across years and added street and housenumber
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F985A1F6-DA54-6B41-930C-3F1383FE14F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936B9113-8E29-A543-A7F2-880C179DF0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29400" yWindow="-7260" windowWidth="23560" windowHeight="21100" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>NNSS</t>
   </si>
@@ -162,6 +162,36 @@
   </si>
   <si>
     <t>756.0000.000.004</t>
+  </si>
+  <si>
+    <t>HAUSNR</t>
+  </si>
+  <si>
+    <t>STRASSE</t>
+  </si>
+  <si>
+    <t>Ackerstrasse</t>
+  </si>
+  <si>
+    <t>Bertastrasse</t>
+  </si>
+  <si>
+    <t>Clausiensteig</t>
+  </si>
+  <si>
+    <t>3c</t>
+  </si>
+  <si>
+    <t>Dammweg</t>
+  </si>
+  <si>
+    <t>Erismannstrasse</t>
+  </si>
+  <si>
+    <t>Floragasse</t>
+  </si>
+  <si>
+    <t>6 f</t>
   </si>
 </sst>
 </file>
@@ -532,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -546,9 +576,10 @@
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -577,22 +608,28 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:16">
       <c r="A2" s="3">
         <v>7560000000001</v>
       </c>
@@ -620,23 +657,29 @@
       <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="J2">
+      <c r="J2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
         <v>804500</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>23</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
       </c>
       <c r="N2">
         <v>0</v>
       </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:16">
       <c r="A3" s="3">
         <v>7560000000002</v>
       </c>
@@ -664,23 +707,29 @@
       <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="J3">
+      <c r="J3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K3">
+        <v>22</v>
+      </c>
+      <c r="L3">
         <v>880200</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>24</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <v>10000</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>1</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:16">
       <c r="A4" s="3">
         <v>7560000000003</v>
       </c>
@@ -705,22 +754,28 @@
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" s="5">
         <v>830200</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>20000</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:16">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -730,8 +785,14 @@
       <c r="C6" t="s">
         <v>36</v>
       </c>
+      <c r="J6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:16">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -741,8 +802,14 @@
       <c r="C7" t="s">
         <v>38</v>
       </c>
+      <c r="J7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7">
+        <v>505</v>
+      </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -751,6 +818,12 @@
       </c>
       <c r="C8" t="s">
         <v>39</v>
+      </c>
+      <c r="J8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed column class in keytable to all character for easier appending
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936B9113-8E29-A543-A7F2-880C179DF0B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C74DDA-35DF-6245-9BD4-2F3F73B72389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-7260" windowWidth="23560" windowHeight="21100" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="29400" yWindow="-7260" windowWidth="34600" windowHeight="21100" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>NNSS</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>6 f</t>
+  </si>
+  <si>
+    <t>STEUERBARESEINKOMMEN</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
   </si>
 </sst>
 </file>
@@ -562,10 +568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -579,7 +585,7 @@
     <col min="10" max="11" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,13 +629,19 @@
         <v>11</v>
       </c>
       <c r="O1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="R1" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:18">
       <c r="A2" s="3">
         <v>7560000000001</v>
       </c>
@@ -678,8 +690,14 @@
       <c r="P2">
         <v>0</v>
       </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>-30</v>
+      </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:18">
       <c r="A3" s="3">
         <v>7560000000002</v>
       </c>
@@ -723,13 +741,19 @@
         <v>10000</v>
       </c>
       <c r="O3">
+        <v>20000000</v>
+      </c>
+      <c r="P3">
         <v>1</v>
       </c>
-      <c r="P3">
+      <c r="Q3">
         <v>0</v>
       </c>
+      <c r="R3">
+        <v>50000</v>
+      </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:18">
       <c r="A4" s="3">
         <v>7560000000003</v>
       </c>
@@ -769,13 +793,16 @@
       <c r="N4">
         <v>20000</v>
       </c>
+      <c r="O4">
+        <v>120003</v>
+      </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:18">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -791,8 +818,14 @@
       <c r="K6">
         <v>4</v>
       </c>
+      <c r="O6">
+        <v>25000</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -808,8 +841,14 @@
       <c r="K7">
         <v>505</v>
       </c>
+      <c r="O7">
+        <v>500000</v>
+      </c>
+      <c r="R7">
+        <v>3600</v>
+      </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -824,6 +863,12 @@
       </c>
       <c r="K8" t="s">
         <v>51</v>
+      </c>
+      <c r="O8">
+        <v>50000</v>
+      </c>
+      <c r="R8">
+        <v>1200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created family Ackermann to test new variable dossier_id
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C74DDA-35DF-6245-9BD4-2F3F73B72389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{659EA295-77BB-B843-A7B4-5E33AC597372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-7260" windowWidth="34600" windowHeight="21100" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="1060" yWindow="740" windowWidth="28340" windowHeight="18380" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
   <si>
     <t>NNSS</t>
   </si>
@@ -198,6 +198,24 @@
   </si>
   <si>
     <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>EGID</t>
+  </si>
+  <si>
+    <t>EWID</t>
+  </si>
+  <si>
+    <t>Anton</t>
+  </si>
+  <si>
+    <t>Anita</t>
+  </si>
+  <si>
+    <t>Civil stat#B</t>
+  </si>
+  <si>
+    <t>Ackermann-Abegger</t>
   </si>
 </sst>
 </file>
@@ -568,16 +586,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
-  <dimension ref="A1:R8"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -585,7 +603,7 @@
     <col min="10" max="11" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -626,22 +644,28 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:20">
       <c r="A2" s="3">
         <v>7560000000001</v>
       </c>
@@ -658,7 +682,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
@@ -682,10 +706,10 @@
         <v>23</v>
       </c>
       <c r="N2">
-        <v>0</v>
+        <v>77777</v>
       </c>
       <c r="O2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -694,10 +718,16 @@
         <v>0</v>
       </c>
       <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
         <v>-30</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="3" spans="1:20">
       <c r="A3" s="3">
         <v>7560000000002</v>
       </c>
@@ -714,7 +744,7 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -738,22 +768,28 @@
         <v>24</v>
       </c>
       <c r="N3">
+        <v>6666</v>
+      </c>
+      <c r="O3">
+        <v>11</v>
+      </c>
+      <c r="P3">
         <v>10000</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>20000000</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>1</v>
       </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
+      <c r="S3">
+        <v>0</v>
+      </c>
+      <c r="T3">
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:20">
       <c r="A4" s="3">
         <v>7560000000003</v>
       </c>
@@ -790,19 +826,25 @@
       <c r="M4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="5">
+        <v>9999999</v>
+      </c>
+      <c r="O4" s="5">
+        <v>999</v>
+      </c>
+      <c r="P4">
         <v>20000</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>120003</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:20">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -818,14 +860,14 @@
       <c r="K6">
         <v>4</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>25000</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:20">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -841,14 +883,14 @@
       <c r="K7">
         <v>505</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>500000</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>3600</v>
       </c>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -864,11 +906,135 @@
       <c r="K8" t="s">
         <v>51</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>50000</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>1200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="3">
+        <v>7560000000007</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="4">
+        <v>34940</v>
+      </c>
+      <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>21</v>
+      </c>
+      <c r="J9" t="s">
+        <v>44</v>
+      </c>
+      <c r="K9">
+        <v>11</v>
+      </c>
+      <c r="L9">
+        <v>804500</v>
+      </c>
+      <c r="M9" t="s">
+        <v>23</v>
+      </c>
+      <c r="N9">
+        <v>77777</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="3">
+        <v>7560000000008</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="4">
+        <v>34940</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10">
+        <v>11</v>
+      </c>
+      <c r="L10">
+        <v>804500</v>
+      </c>
+      <c r="M10" t="s">
+        <v>23</v>
+      </c>
+      <c r="N10">
+        <v>77777</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>-30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new function to create id for people with same address and same last name
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{659EA295-77BB-B843-A7B4-5E33AC597372}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC70D0A-0383-3049-9792-5A2FBB26F92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="740" windowWidth="28340" windowHeight="18380" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
   <si>
     <t>NNSS</t>
   </si>
@@ -179,9 +179,6 @@
     <t>Clausiensteig</t>
   </si>
   <si>
-    <t>3c</t>
-  </si>
-  <si>
     <t>Dammweg</t>
   </si>
   <si>
@@ -212,10 +209,25 @@
     <t>Anita</t>
   </si>
   <si>
-    <t>Civil stat#B</t>
-  </si>
-  <si>
     <t>Ackermann-Abegger</t>
+  </si>
+  <si>
+    <t>31.02.1965</t>
+  </si>
+  <si>
+    <t>Apmann</t>
+  </si>
+  <si>
+    <t>Ali</t>
+  </si>
+  <si>
+    <t>CHResidenc#L</t>
+  </si>
+  <si>
+    <t>Civil stat#M</t>
+  </si>
+  <si>
+    <t>3c!</t>
   </si>
 </sst>
 </file>
@@ -586,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -644,16 +656,16 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>12</v>
@@ -662,7 +674,7 @@
         <v>13</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:20">
@@ -682,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
         <v>20</v>
@@ -818,7 +830,7 @@
         <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="L4" s="5">
         <v>830200</v>
@@ -855,7 +867,7 @@
         <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K6">
         <v>4</v>
@@ -878,7 +890,7 @@
         <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K7">
         <v>505</v>
@@ -901,10 +913,10 @@
         <v>39</v>
       </c>
       <c r="J8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K8" t="s">
         <v>50</v>
-      </c>
-      <c r="K8" t="s">
-        <v>51</v>
       </c>
       <c r="Q8">
         <v>50000</v>
@@ -921,16 +933,16 @@
         <v>29</v>
       </c>
       <c r="C9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="4">
-        <v>34940</v>
+        <v>55</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="E9" t="s">
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G9" t="s">
         <v>18</v>
@@ -980,19 +992,19 @@
         <v>7560000000008</v>
       </c>
       <c r="B10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D10" s="4">
-        <v>34940</v>
+        <v>26320</v>
       </c>
       <c r="E10" t="s">
         <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="G10" t="s">
         <v>19</v>
@@ -1034,6 +1046,68 @@
         <v>0</v>
       </c>
       <c r="T10">
+        <v>-30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="3">
+        <v>7560000000009</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="4">
+        <v>30246</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" t="s">
+        <v>44</v>
+      </c>
+      <c r="K11">
+        <v>11</v>
+      </c>
+      <c r="L11">
+        <v>804500</v>
+      </c>
+      <c r="M11" t="s">
+        <v>23</v>
+      </c>
+      <c r="N11">
+        <v>77777</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
         <v>-30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
create household id approximation
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC70D0A-0383-3049-9792-5A2FBB26F92E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EAFB4E-FEF7-F148-B130-872A5AAEDF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="740" windowWidth="28340" windowHeight="18380" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="1060" yWindow="660" windowWidth="24540" windowHeight="15980" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1093,7 +1093,7 @@
         <v>77777</v>
       </c>
       <c r="O11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11">
         <v>0</v>

</xml_diff>

<commit_message>
created sip with 4 digits to export in PANON and Address
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81EAFB4E-FEF7-F148-B130-872A5AAEDF32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C74DDA-35DF-6245-9BD4-2F3F73B72389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="660" windowWidth="24540" windowHeight="15980" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="29400" yWindow="-7260" windowWidth="34600" windowHeight="21100" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>NNSS</t>
   </si>
@@ -179,6 +179,9 @@
     <t>Clausiensteig</t>
   </si>
   <si>
+    <t>3c</t>
+  </si>
+  <si>
     <t>Dammweg</t>
   </si>
   <si>
@@ -195,39 +198,6 @@
   </si>
   <si>
     <t>AMOUNT</t>
-  </si>
-  <si>
-    <t>EGID</t>
-  </si>
-  <si>
-    <t>EWID</t>
-  </si>
-  <si>
-    <t>Anton</t>
-  </si>
-  <si>
-    <t>Anita</t>
-  </si>
-  <si>
-    <t>Ackermann-Abegger</t>
-  </si>
-  <si>
-    <t>31.02.1965</t>
-  </si>
-  <si>
-    <t>Apmann</t>
-  </si>
-  <si>
-    <t>Ali</t>
-  </si>
-  <si>
-    <t>CHResidenc#L</t>
-  </si>
-  <si>
-    <t>Civil stat#M</t>
-  </si>
-  <si>
-    <t>3c!</t>
   </si>
 </sst>
 </file>
@@ -598,16 +568,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
-  <dimension ref="A1:T11"/>
+  <dimension ref="A1:R8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="28.83203125" customWidth="1"/>
-    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
@@ -615,7 +585,7 @@
     <col min="10" max="11" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -656,28 +626,22 @@
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>52</v>
-      </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:18">
       <c r="A2" s="3">
         <v>7560000000001</v>
       </c>
@@ -718,10 +682,10 @@
         <v>23</v>
       </c>
       <c r="N2">
-        <v>77777</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
         <v>0</v>
@@ -730,16 +694,10 @@
         <v>0</v>
       </c>
       <c r="R2">
-        <v>0</v>
-      </c>
-      <c r="S2">
-        <v>0</v>
-      </c>
-      <c r="T2">
         <v>-30</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:18">
       <c r="A3" s="3">
         <v>7560000000002</v>
       </c>
@@ -756,7 +714,7 @@
         <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
         <v>19</v>
@@ -780,28 +738,22 @@
         <v>24</v>
       </c>
       <c r="N3">
-        <v>6666</v>
+        <v>10000</v>
       </c>
       <c r="O3">
-        <v>11</v>
+        <v>20000000</v>
       </c>
       <c r="P3">
-        <v>10000</v>
+        <v>1</v>
       </c>
       <c r="Q3">
-        <v>20000000</v>
+        <v>0</v>
       </c>
       <c r="R3">
-        <v>1</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
         <v>50000</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:18">
       <c r="A4" s="3">
         <v>7560000000003</v>
       </c>
@@ -830,7 +782,7 @@
         <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="L4" s="5">
         <v>830200</v>
@@ -838,25 +790,19 @@
       <c r="M4" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="5">
-        <v>9999999</v>
-      </c>
-      <c r="O4" s="5">
-        <v>999</v>
-      </c>
-      <c r="P4">
+      <c r="N4">
         <v>20000</v>
       </c>
-      <c r="Q4">
+      <c r="O4">
         <v>120003</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:18">
       <c r="A6" s="3" t="s">
         <v>41</v>
       </c>
@@ -867,19 +813,19 @@
         <v>36</v>
       </c>
       <c r="J6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K6">
         <v>4</v>
       </c>
-      <c r="Q6">
+      <c r="O6">
         <v>25000</v>
       </c>
-      <c r="T6">
+      <c r="R6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:18">
       <c r="A7" s="3" t="s">
         <v>33</v>
       </c>
@@ -890,19 +836,19 @@
         <v>38</v>
       </c>
       <c r="J7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K7">
         <v>505</v>
       </c>
-      <c r="Q7">
+      <c r="O7">
         <v>500000</v>
       </c>
-      <c r="T7">
+      <c r="R7">
         <v>3600</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -913,202 +859,16 @@
         <v>39</v>
       </c>
       <c r="J8" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K8" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q8">
+        <v>51</v>
+      </c>
+      <c r="O8">
         <v>50000</v>
       </c>
-      <c r="T8">
+      <c r="R8">
         <v>1200</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20">
-      <c r="A9" s="3">
-        <v>7560000000007</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="H9">
-        <v>3</v>
-      </c>
-      <c r="I9" t="s">
-        <v>21</v>
-      </c>
-      <c r="J9" t="s">
-        <v>44</v>
-      </c>
-      <c r="K9">
-        <v>11</v>
-      </c>
-      <c r="L9">
-        <v>804500</v>
-      </c>
-      <c r="M9" t="s">
-        <v>23</v>
-      </c>
-      <c r="N9">
-        <v>77777</v>
-      </c>
-      <c r="O9">
-        <v>1</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-      <c r="R9">
-        <v>0</v>
-      </c>
-      <c r="S9">
-        <v>0</v>
-      </c>
-      <c r="T9">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" s="3">
-        <v>7560000000008</v>
-      </c>
-      <c r="B10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D10" s="4">
-        <v>26320</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H10">
-        <v>3</v>
-      </c>
-      <c r="I10" t="s">
-        <v>21</v>
-      </c>
-      <c r="J10" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10">
-        <v>11</v>
-      </c>
-      <c r="L10">
-        <v>804500</v>
-      </c>
-      <c r="M10" t="s">
-        <v>23</v>
-      </c>
-      <c r="N10">
-        <v>77777</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>-30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="A11" s="3">
-        <v>7560000000009</v>
-      </c>
-      <c r="B11" t="s">
-        <v>59</v>
-      </c>
-      <c r="C11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="4">
-        <v>30246</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="H11">
-        <v>3</v>
-      </c>
-      <c r="I11" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11">
-        <v>11</v>
-      </c>
-      <c r="L11">
-        <v>804500</v>
-      </c>
-      <c r="M11" t="s">
-        <v>23</v>
-      </c>
-      <c r="N11">
-        <v>77777</v>
-      </c>
-      <c r="O11">
-        <v>2</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>0</v>
-      </c>
-      <c r="R11">
-        <v>0</v>
-      </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
-      <c r="T11">
-        <v>-30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
autodetect and execute csv import
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF06A0C-1227-E741-8918-F267DFF984E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879096AC-E6EF-AE4F-B788-67339B8E541B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="660" windowWidth="24580" windowHeight="15980" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
+    <workbookView xWindow="1080" yWindow="740" windowWidth="24580" windowHeight="15980" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -253,13 +252,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -576,8 +579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -589,6 +592,7 @@
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="23.1640625" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -625,7 +629,7 @@
       <c r="K1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -687,7 +691,7 @@
       <c r="K2">
         <v>11</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="8">
         <v>804500</v>
       </c>
       <c r="M2" t="s">
@@ -749,7 +753,7 @@
       <c r="K3">
         <v>22</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="8">
         <v>880200</v>
       </c>
       <c r="M3" t="s">
@@ -808,7 +812,7 @@
       <c r="K4" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L4" s="9">
         <v>830200</v>
       </c>
       <c r="M4" s="5" t="s">
@@ -851,6 +855,9 @@
       <c r="K6">
         <v>4</v>
       </c>
+      <c r="L6" s="6">
+        <v>8.9999999999999996E+22</v>
+      </c>
       <c r="Q6">
         <v>25000</v>
       </c>
@@ -873,6 +880,9 @@
       </c>
       <c r="K7">
         <v>505</v>
+      </c>
+      <c r="L7" s="8">
+        <v>200</v>
       </c>
       <c r="Q7">
         <v>500000</v>

</xml_diff>

<commit_message>
dynamic egid and ewid
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879096AC-E6EF-AE4F-B788-67339B8E541B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACD0E13-BD9B-364F-A8AF-2ED575B8EC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="740" windowWidth="24580" windowHeight="15980" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
@@ -252,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -260,9 +260,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -592,7 +589,6 @@
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="23.1640625" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -629,7 +625,7 @@
       <c r="K1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -691,7 +687,7 @@
       <c r="K2">
         <v>11</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2">
         <v>804500</v>
       </c>
       <c r="M2" t="s">
@@ -753,7 +749,7 @@
       <c r="K3">
         <v>22</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3">
         <v>880200</v>
       </c>
       <c r="M3" t="s">
@@ -812,14 +808,14 @@
       <c r="K4" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="5">
         <v>830200</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>25</v>
       </c>
       <c r="N4" s="5">
-        <v>9999999</v>
+        <v>999999999</v>
       </c>
       <c r="O4" s="5">
         <v>999</v>
@@ -881,7 +877,7 @@
       <c r="K7">
         <v>505</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7">
         <v>200</v>
       </c>
       <c r="Q7">

</xml_diff>

<commit_message>
replace ewid_ and egid_pseudo with 999999999 to follow BFS code for people who cannot be assigned to a cell
</commit_message>
<xml_diff>
--- a/data-raw/FAKE_DATA_2019.xlsx
+++ b/data-raw/FAKE_DATA_2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/flhug/Dropbox (Personal)/PhD/Courses/H4Sci_Project/Git/pseudonymizer/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879096AC-E6EF-AE4F-B788-67339B8E541B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7C364A-38EC-1245-969F-89F058F197A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="740" windowWidth="24580" windowHeight="15980" xr2:uid="{F2FEE1B5-A181-9D49-99C5-546F0817DC33}"/>
   </bookViews>
@@ -252,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -260,9 +260,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BF7B3D-EBD7-8C4D-A454-F3444C20C8ED}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -592,7 +589,6 @@
     <col min="8" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="23.1640625" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20">
@@ -629,7 +625,7 @@
       <c r="K1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -691,7 +687,7 @@
       <c r="K2">
         <v>11</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2">
         <v>804500</v>
       </c>
       <c r="M2" t="s">
@@ -753,7 +749,7 @@
       <c r="K3">
         <v>22</v>
       </c>
-      <c r="L3" s="8">
+      <c r="L3">
         <v>880200</v>
       </c>
       <c r="M3" t="s">
@@ -812,14 +808,14 @@
       <c r="K4" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="9">
+      <c r="L4" s="5">
         <v>830200</v>
       </c>
       <c r="M4" s="5" t="s">
         <v>25</v>
       </c>
       <c r="N4" s="5">
-        <v>9999999</v>
+        <v>999999999</v>
       </c>
       <c r="O4" s="5">
         <v>999</v>
@@ -881,7 +877,7 @@
       <c r="K7">
         <v>505</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7">
         <v>200</v>
       </c>
       <c r="Q7">

</xml_diff>